<commit_message>
fix for geography data structure
</commit_message>
<xml_diff>
--- a/meltexapp/seeding/seed_data/seed_data.xlsx
+++ b/meltexapp/seeding/seed_data/seed_data.xlsx
@@ -791,13 +791,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1125,7 +1125,7 @@
         <v>206</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>208</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>207</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>209</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>207</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>211</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>211</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>213</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>211</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>211</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>215</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>216</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
         <v>215</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
         <v>215</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>218</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
         <v>215</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>219</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>215</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>220</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>221</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
         <v>220</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>222</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
         <v>220</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
         <v>220</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>224</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
         <v>220</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>225</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3" t="s">
         <v>220</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3" t="s">
         <v>220</v>
       </c>

</xml_diff>